<commit_message>
Version und Datum hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumentation/Terminplan.xlsx
+++ b/Dokumentation/Terminplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F33F5C-ADBF-4B51-967E-EBD483A6B530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D03B52-4530-4010-A1FE-C860F67D92EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Titel für die einzelnen Ergebnisse der oben dargestellten Phasen sind in dieser Zeile von Zelle C13 bis F13 aufgeführt.
 Überschreiben oder löschen Sie die Beispieldaten, um Ihre eigenen Titel zu erstellen.</t>
@@ -432,6 +432,15 @@
     <t>• Konzept für Kommunikation zwischen PC und Arduino entwerfen
 • GUI mit 6 Buttons entwickeln, jeder Button schickt per UART ein Code an das Arduino
 • Unittest für eine Funktion implementieren</t>
+  </si>
+  <si>
+    <t>Datum:</t>
+  </si>
+  <si>
+    <t>Version:</t>
+  </si>
+  <si>
+    <t>1.1</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1252,7 @@
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -1366,6 +1375,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1727,7 +1745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF5989AE-1305-4647-BBA5-100DFF61C1D5}" type="CELLRANGE">
+                    <a:fld id="{76C3E28D-F1A4-4DDD-914F-38A1B58F07FF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1760,7 +1778,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B095C6E3-41AF-4F58-9EB2-AC950EA2C9CE}" type="CELLRANGE">
+                    <a:fld id="{18682523-B2C2-4B13-91A1-DAD99258D63B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1826,7 +1844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C3C2651-D8C5-4C3A-AE54-B044D2E30091}" type="CELLRANGE">
+                    <a:fld id="{6D60AABD-BD6A-4C73-908D-A1256A96D679}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1859,7 +1877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EA61826-B8C8-4A71-8F98-D06C1EE0BCF7}" type="CELLRANGE">
+                    <a:fld id="{47575D8D-B8BE-47DF-929F-A28F7CAC3F39}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1930,7 +1948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4751EA4-E64E-4B2D-9885-836E7BC6BF35}" type="CELLRANGE">
+                    <a:fld id="{1360D7DA-D397-42E9-8497-68328930BCB5}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -3523,7 +3541,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3838,25 +3856,37 @@
       </c>
       <c r="H16" s="42"/>
     </row>
-    <row r="18" spans="3:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C19" s="25" t="s">
         <v>64</v>
       </c>
       <c r="D19" s="24"/>
     </row>
-    <row r="20" spans="3:4" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="26" t="s">
         <v>42</v>
       </c>
+      <c r="G20" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="44">
+        <v>43766</v>
+      </c>
     </row>
-    <row r="21" spans="3:4" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C21" s="26" t="s">
         <v>43</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
geschätzer Aufwand, Resourcen und Dauer eingefügt, wie von Modulleiter Herr Trummer gefordert, erneut zur Abgabe geschickt
</commit_message>
<xml_diff>
--- a/Dokumentation/Terminplan.xlsx
+++ b/Dokumentation/Terminplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A31F3F8-BE26-446E-BCCA-A6CD383C1CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57C365A-697F-4870-9FDD-EE030D3F7592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Titel für die einzelnen Ergebnisse der oben dargestellten Phasen sind in dieser Zeile von Zelle C13 bis F13 aufgeführt.
 Überschreiben oder löschen Sie die Beispieldaten, um Ihre eigenen Titel zu erstellen.</t>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Phase 3</t>
-  </si>
-  <si>
-    <t>Phase 4</t>
   </si>
   <si>
     <t>Namen:</t>
@@ -495,24 +492,51 @@
     </r>
   </si>
   <si>
-    <t>1.2</t>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>geschätzer Aufwand</t>
+  </si>
+  <si>
+    <t>Ist Aufwand</t>
+  </si>
+  <si>
+    <t>Resoucen (gerechnet auf 40 Std-Woche)</t>
+  </si>
+  <si>
+    <t>geschätze Dauer</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>angepasster Terminplan abgegeben</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="[$-407]d\.\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="173" formatCode="0.0\ &quot;Wochen&quot;"/>
+    <numFmt numFmtId="175" formatCode="0\ \ &quot;Stunden&quot;"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -762,7 +786,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -960,8 +984,20 @@
         <bgColor theme="0" tint="-4.9989318521683403E-2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1055,21 +1091,6 @@
       </left>
       <right style="double">
         <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
       </right>
       <top style="thin">
         <color theme="3" tint="0.39994506668294322"/>
@@ -1210,36 +1231,6 @@
       <left style="double">
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
-      <right style="double">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
       <right style="thin">
         <color theme="4" tint="0.39994506668294322"/>
       </right>
@@ -1273,174 +1264,369 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1455,16 +1641,94 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="1" fillId="37" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="1" fillId="37" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1849,6 +2113,21 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-D147-4342-85F7-92EE1B94B803}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -1857,7 +2136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{279922D4-20DE-45EA-A654-FE2FF1E62CF6}" type="CELLRANGE">
+                    <a:fld id="{FBC82E5D-5C2D-42C0-8C29-F2B22EC46F18}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1890,7 +2169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18F4AD6F-989B-49D7-AA3D-27A2A3DF556E}" type="CELLRANGE">
+                    <a:fld id="{33E4A0BC-7EB9-4E1D-9EB7-E857ED1F6A3C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1923,7 +2202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD68E4D5-B2BC-4ACA-A1F9-74E7F4340996}" type="CELLRANGE">
+                    <a:fld id="{3F15AD05-3093-4790-BF4E-7A6BB139AC5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1956,7 +2235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CECC972-7865-4A84-9681-CC06982F0C0B}" type="CELLRANGE">
+                    <a:fld id="{253DAEF6-7AF9-4EA1-812D-ED6EAA907327}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1989,7 +2268,40 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A4DB539-6920-40DC-9C9D-5A5E33227A98}" type="CELLRANGE">
+                    <a:fld id="{5CE501DF-5195-4664-ACB7-5C94A69CCF3A}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-D147-4342-85F7-92EE1B94B803}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{EA1BE266-518F-4604-B935-ED891CFF236B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2011,39 +2323,6 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-D147-4342-85F7-92EE1B94B803}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{0F23B767-0734-48D0-B13A-CBE5DD07F33C}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-D147-4342-85F7-92EE1B94B803}"/>
                 </c:ext>
               </c:extLst>
@@ -2055,7 +2334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4894A311-9547-43AC-83D2-ABD68E347B0C}" type="CELLRANGE">
+                    <a:fld id="{125EE923-22CD-483D-82F8-FB4A80681F51}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2083,50 +2362,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.7069459958426979E-2"/>
-                  <c:y val="1.3139500993451975E-16"/>
-                </c:manualLayout>
-              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7ED23839-339E-43D9-BC54-5508192850A6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-D147-4342-85F7-92EE1B94B803}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{EED6BBE2-BAE7-4D02-9988-969419E327F7}" type="CELLRANGE">
+                    <a:fld id="{D2BFDC71-853D-441C-A610-2F4DE50D6E0C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2148,16 +2389,16 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-FF47-45C8-A0A4-F2821B199328}"/>
+                  <c16:uniqueId val="{00000007-D147-4342-85F7-92EE1B94B803}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="9"/>
+              <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.3220222068248076E-4"/>
-                  <c:y val="7.167083335684739E-3"/>
+                  <c:x val="-1.7069459958426979E-2"/>
+                  <c:y val="1.3139500993451975E-16"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2165,7 +2406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5F91CAC-2F3E-4CAF-9C7F-6E296E236015}" type="CELLRANGE">
+                    <a:fld id="{308EB7F1-46D2-4D1E-958A-AF29BC74DE96}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2186,7 +2427,75 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-FF47-45C8-A0A4-F2821B199328}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{95815A99-8559-476A-9805-0997801F9639}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-8301-4D89-AB66-D71705F6B622}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.3220222068248076E-4"/>
+                  <c:y val="7.167083335684739E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FFFA1F33-0865-4DEE-B299-9613A07D58E4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ZELLBEREICH]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2219,9 +2528,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Zeitachse-Daten'!$B$3:$B$12</c:f>
+              <c:f>'Zeitachse-Daten'!$B$3:$B$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Projektanfang</c:v>
                 </c:pt>
@@ -2235,21 +2544,24 @@
                   <c:v>Terminplan abgegeben</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>angepasster Terminplan abgegeben</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Abgabetermin Terminplan</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Meilenstein 1: Mussanforderungen umgesetzt</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Meilenstein 2: Sollanforderungen umgesetzt</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Meilenstein 3: Wunschanforderungen umgesetzt</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Präsentation Projekt</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Abgabetermin Code &amp; Projektende</c:v>
                 </c:pt>
               </c:strCache>
@@ -2257,10 +2569,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Zeitachse-Daten'!$C$3:$C$12</c:f>
+              <c:f>'Zeitachse-Daten'!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -2274,21 +2586,24 @@
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -2297,9 +2612,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>'Zeitachse-Daten'!$B$3:$B$12</c15:f>
+                <c15:f>'Zeitachse-Daten'!$B$3:$B$13</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="11"/>
                   <c:pt idx="0">
                     <c:v>Projektanfang</c:v>
                   </c:pt>
@@ -2313,21 +2628,24 @@
                     <c:v>Terminplan abgegeben</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>angepasster Terminplan abgegeben</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Abgabetermin Terminplan</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Meilenstein 1: Mussanforderungen umgesetzt</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>Meilenstein 2: Sollanforderungen umgesetzt</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>Meilenstein 3: Wunschanforderungen umgesetzt</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>Präsentation Projekt</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>Abgabetermin Code &amp; Projektende</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
@@ -2395,10 +2713,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'Zeitachse-Daten'!$A$3:$A$12</c:f>
+              <c:f>'Zeitachse-Daten'!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>[$-407]d\.\ mmmm\ yyyy;@</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43734</c:v>
                 </c:pt>
@@ -2412,21 +2730,24 @@
                   <c:v>43766</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>43779</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43783</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43797</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43811</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43818</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43821</c:v>
                 </c:pt>
               </c:numCache>
@@ -2434,10 +2755,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Zeitachse-Daten'!$D$3:$D$12</c:f>
+              <c:f>'Zeitachse-Daten'!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2466,6 +2787,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2785,115 +3109,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19034</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9527</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2886069</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>942977</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Pfeil: Chevron 7" descr="Arrow containing title &quot;Phase 4&quot;. Project phase activities and outcomes are listed in this column, below the arrow.">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A31CBE6-B921-47FA-B959-6267109C7392}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9377347" y="704852"/>
-          <a:ext cx="2867035" cy="933450"/>
-        </a:xfrm>
-        <a:prstGeom prst="chevron">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0"/>
-          <a:endParaRPr lang="en-US" sz="1800">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0"/>
-          <a:r>
-            <a:rPr lang="de" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Phase</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de" sz="1800" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> 4</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1800">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2904,7 +3119,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2971,13 +3186,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>774703</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3039,10 +3254,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3035300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9527</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3200400" cy="933450"/>
     <xdr:sp macro="" textlink="">
@@ -3058,7 +3273,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12077700" y="4264027"/>
+          <a:off x="12141200" y="4762500"/>
           <a:ext cx="3200400" cy="933450"/>
         </a:xfrm>
         <a:prstGeom prst="chevron">
@@ -3386,7 +3601,7 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>680</xdr:rowOff>
@@ -3420,8 +3635,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB69B43E-2BA1-4B78-B847-BBD11421F13E}" name="Aktivitäten" displayName="Aktivitäten" ref="B6:F11">
-  <autoFilter ref="B6:F11" xr:uid="{53A827E8-F9FA-44B0-9C5C-0FC3323461F0}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB69B43E-2BA1-4B78-B847-BBD11421F13E}" name="Aktivitäten" displayName="Aktivitäten" ref="B6:F27">
+  <autoFilter ref="B6:F27" xr:uid="{53A827E8-F9FA-44B0-9C5C-0FC3323461F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3433,7 +3648,7 @@
     <tableColumn id="2" xr3:uid="{1F14BBD8-81A4-412A-9781-543247F1EE96}" name="Namen:"/>
     <tableColumn id="3" xr3:uid="{42DF497C-052C-4DD7-A4FA-DAE97DBD28F3}" name="Pflichtenheft &amp; Projektplan erstellen"/>
     <tableColumn id="4" xr3:uid="{914C0B14-DD22-4A67-9ECC-BF1062B7054B}" name="  "/>
-    <tableColumn id="5" xr3:uid="{1D5922C5-D2F9-4D6C-B0EF-C247CCD4B6D6}" name="   " totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1D5922C5-D2F9-4D6C-B0EF-C247CCD4B6D6}" name="   " totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Activities table style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
   <extLst>
@@ -3445,8 +3660,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD5620BB-7EAF-4160-89F5-4456ED11BB1D}" name="Ergebnisse" displayName="Ergebnisse" ref="B13:F18">
-  <autoFilter ref="B13:F18" xr:uid="{767D240A-8DEC-4020-8CBB-200F1CAFCDF4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AD5620BB-7EAF-4160-89F5-4456ED11BB1D}" name="Ergebnisse" displayName="Ergebnisse" ref="B29:F34">
+  <autoFilter ref="B29:F34" xr:uid="{767D240A-8DEC-4020-8CBB-200F1CAFCDF4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3458,7 +3673,7 @@
     <tableColumn id="2" xr3:uid="{22FE4A6A-9AAB-49E5-B8B6-9976E3D4735D}" name="Namen:"/>
     <tableColumn id="3" xr3:uid="{BCC79B64-076D-42FF-B72F-ED7A8ED5A607}" name="  "/>
     <tableColumn id="4" xr3:uid="{C4A793C0-C514-4A82-BFEB-5CF7C3AAE498}" name="1. Prototyp fertig"/>
-    <tableColumn id="5" xr3:uid="{B2A1622D-5883-4114-A1A3-40EDE66A747B}" name="2. Protoyp fertig" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B2A1622D-5883-4114-A1A3-40EDE66A747B}" name="2. Protoyp fertig" totalsRowFunction="count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Outcomes table style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
   <extLst>
@@ -3736,10 +3951,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3751,12 +3966,13 @@
     <col min="5" max="6" width="40.58203125" customWidth="1"/>
     <col min="7" max="7" width="43.4140625" customWidth="1"/>
     <col min="8" max="8" width="29.9140625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="C1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -3764,7 +3980,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="279.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="279.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -3773,20 +3989,20 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>74</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>75</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -3795,7 +4011,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -3804,34 +4020,32 @@
       <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -3846,276 +4060,633 @@
       <c r="F7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="42" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="59">
+        <v>1</v>
+      </c>
+      <c r="E9" s="59">
+        <v>9</v>
+      </c>
+      <c r="F9" s="59">
+        <v>6</v>
+      </c>
+      <c r="G9" s="60">
+        <v>6</v>
+      </c>
+      <c r="H9" s="61">
+        <v>2</v>
+      </c>
+      <c r="I9" s="63">
+        <f>SUM(D9:H9)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="59">
+        <v>1</v>
+      </c>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G11" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="48">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="50">
+        <f xml:space="preserve"> D9/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="50">
+        <f xml:space="preserve"> E9/2</f>
+        <v>4.5</v>
+      </c>
+      <c r="F12" s="50">
+        <f xml:space="preserve"> F9/2</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="51">
+        <f xml:space="preserve"> G9/2</f>
+        <v>3</v>
+      </c>
+      <c r="H12" s="52">
+        <f xml:space="preserve"> H9/2</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="64">
+        <f>SUM(D12:H12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="59">
+        <v>1</v>
+      </c>
+      <c r="E14" s="59">
+        <v>12</v>
+      </c>
+      <c r="F14" s="59">
+        <v>2</v>
+      </c>
+      <c r="G14" s="60">
+        <v>2</v>
+      </c>
+      <c r="H14" s="61">
+        <v>3</v>
+      </c>
+      <c r="I14" s="63">
+        <f>SUM(D14:H14)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="59">
+        <v>1</v>
+      </c>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="E16" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="H16" s="48">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="50">
+        <f xml:space="preserve"> D14/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="50">
+        <f xml:space="preserve"> E14/2</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="50">
+        <f xml:space="preserve"> F14/2</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="51">
+        <f xml:space="preserve"> G14/2</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="52">
+        <f xml:space="preserve"> H14/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="I17" s="64">
+        <f>SUM(D17:H17)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="59">
+        <v>8</v>
+      </c>
+      <c r="E19" s="59">
+        <v>2</v>
+      </c>
+      <c r="F19" s="59">
+        <v>4</v>
+      </c>
+      <c r="G19" s="60">
+        <v>4</v>
+      </c>
+      <c r="H19" s="61">
+        <v>2</v>
+      </c>
+      <c r="I19" s="63">
+        <f>SUM(D19:H19)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="59">
+        <v>10</v>
+      </c>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="61"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="E21" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G21" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="H21" s="48">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="50">
+        <f xml:space="preserve"> D19/2</f>
+        <v>4</v>
+      </c>
+      <c r="E22" s="50">
+        <f xml:space="preserve"> E19/2</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="50">
+        <f xml:space="preserve"> F19/2</f>
+        <v>2</v>
+      </c>
+      <c r="G22" s="51">
+        <f xml:space="preserve"> G19/2</f>
+        <v>2</v>
+      </c>
+      <c r="H22" s="52">
+        <f xml:space="preserve"> H19/2</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="64">
+        <f>SUM(D22:H22)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D23" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E23" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="59">
+        <v>1</v>
+      </c>
+      <c r="E24" s="59">
+        <v>8</v>
+      </c>
+      <c r="F24" s="59">
+        <v>3</v>
+      </c>
+      <c r="G24" s="60">
+        <v>4</v>
+      </c>
+      <c r="H24" s="61">
+        <v>4</v>
+      </c>
+      <c r="I24" s="63">
+        <f>SUM(D24:H24)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="59">
+        <v>1</v>
+      </c>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="E26" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G26" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="H26" s="48">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="50">
+        <f xml:space="preserve"> D24/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="50">
+        <f xml:space="preserve"> E24/2</f>
+        <v>4</v>
+      </c>
+      <c r="F27" s="50">
+        <f xml:space="preserve"> F24/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="51">
+        <f xml:space="preserve"> G24/2</f>
+        <v>2</v>
+      </c>
+      <c r="H27" s="52">
+        <f xml:space="preserve"> H24/2</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="64">
+        <f>SUM(D27:H27)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="36" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C37" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="24"/>
+    </row>
+    <row r="38" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="45"/>
-    </row>
-    <row r="17" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="45"/>
-    </row>
-    <row r="18" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="46"/>
-    </row>
-    <row r="20" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="26" t="s">
+      <c r="H38" s="33">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C39" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G39" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="41">
-        <v>43766</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>76</v>
+      <c r="H39" s="34" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="H31:H34"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="36" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="29" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -4129,10 +4700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612DC874-566E-4E81-9C07-EE9CDBC3E61D}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4146,23 +4717,23 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4171,7 +4742,7 @@
         <v>43734</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="12">
         <v>20</v>
@@ -4185,7 +4756,7 @@
         <v>43746</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12">
         <v>-20</v>
@@ -4200,7 +4771,7 @@
         <v>43751</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="10">
         <v>20</v>
@@ -4214,7 +4785,7 @@
         <v>43766</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="10">
         <v>-20</v>
@@ -4225,109 +4796,123 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
+        <v>43770</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-30</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <f>DATE(2019,11,10)</f>
         <v>43779</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="B8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="10">
         <v>20</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D8" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <f>DATE(2019,11,14)</f>
         <v>43783</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10">
         <v>-20</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D9" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <f>DATE(2019,11,28)</f>
         <v>43797</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10">
         <v>-30</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D10" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <f>DATE(2019,12,12)</f>
         <v>43811</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10">
         <v>-20</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D11" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <f>DATE(2019,12,19)</f>
         <v>43818</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="10">
         <v>-30</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D12" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <f>DATE(2019,12,22)</f>
         <v>43821</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="10">
         <v>20</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D13" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-    </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+      <c r="B17" s="31"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="31"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="4">

</xml_diff>

<commit_message>
Feld fuer Ist-Zeit erstellt
</commit_message>
<xml_diff>
--- a/Dokumentation/Terminplan.xlsx
+++ b/Dokumentation/Terminplan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57C365A-697F-4870-9FDD-EE030D3F7592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D42D7-1974-4905-A527-CE2BDADDE581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
@@ -523,8 +523,8 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="[$-407]d\.\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="173" formatCode="0.0\ &quot;Wochen&quot;"/>
-    <numFmt numFmtId="175" formatCode="0\ \ &quot;Stunden&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.0\ &quot;Wochen&quot;"/>
+    <numFmt numFmtId="170" formatCode="0\ \ &quot;Stunden&quot;"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1644,6 +1644,84 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="37" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="37" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1651,84 +1729,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="1" fillId="37" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="1" fillId="37" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2136,7 +2136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBC82E5D-5C2D-42C0-8C29-F2B22EC46F18}" type="CELLRANGE">
+                    <a:fld id="{21787663-4A21-4442-A1D7-1F1E8A107D74}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2169,7 +2169,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33E4A0BC-7EB9-4E1D-9EB7-E857ED1F6A3C}" type="CELLRANGE">
+                    <a:fld id="{FBF1BAEE-70A3-40A7-8FD5-F944CEE1E780}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2202,7 +2202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F15AD05-3093-4790-BF4E-7A6BB139AC5D}" type="CELLRANGE">
+                    <a:fld id="{6D92D8BA-BA51-41D3-A307-5E6C04F72D3C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2235,7 +2235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{253DAEF6-7AF9-4EA1-812D-ED6EAA907327}" type="CELLRANGE">
+                    <a:fld id="{67C62430-54B0-41C1-AB21-F561D122263D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2268,7 +2268,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CE501DF-5195-4664-ACB7-5C94A69CCF3A}" type="CELLRANGE">
+                    <a:fld id="{D8514844-197C-4B5F-AFA9-C2A738DEB967}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2334,7 +2334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{125EE923-22CD-483D-82F8-FB4A80681F51}" type="CELLRANGE">
+                    <a:fld id="{D46C1F9C-EE3D-462D-850B-C9ED7A618A63}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2367,7 +2367,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2BFDC71-853D-441C-A610-2F4DE50D6E0C}" type="CELLRANGE">
+                    <a:fld id="{09B3B258-18AA-4545-A783-28A0D4DFEF62}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2438,7 +2438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95815A99-8559-476A-9805-0997801F9639}" type="CELLRANGE">
+                    <a:fld id="{5C50F171-2994-4F8C-9818-D6E795E1F43F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2496,6 +2496,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-984C-4F5C-9445-FB4E7CD04C96}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3648,7 +3651,7 @@
     <tableColumn id="2" xr3:uid="{1F14BBD8-81A4-412A-9781-543247F1EE96}" name="Namen:"/>
     <tableColumn id="3" xr3:uid="{42DF497C-052C-4DD7-A4FA-DAE97DBD28F3}" name="Pflichtenheft &amp; Projektplan erstellen"/>
     <tableColumn id="4" xr3:uid="{914C0B14-DD22-4A67-9ECC-BF1062B7054B}" name="  "/>
-    <tableColumn id="5" xr3:uid="{1D5922C5-D2F9-4D6C-B0EF-C247CCD4B6D6}" name="   " totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{1D5922C5-D2F9-4D6C-B0EF-C247CCD4B6D6}" name="   " totalsRowFunction="count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Activities table style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
   <extLst>
@@ -3673,7 +3676,7 @@
     <tableColumn id="2" xr3:uid="{22FE4A6A-9AAB-49E5-B8B6-9976E3D4735D}" name="Namen:"/>
     <tableColumn id="3" xr3:uid="{BCC79B64-076D-42FF-B72F-ED7A8ED5A607}" name="  "/>
     <tableColumn id="4" xr3:uid="{C4A793C0-C514-4A82-BFEB-5CF7C3AAE498}" name="1. Prototyp fertig"/>
-    <tableColumn id="5" xr3:uid="{B2A1622D-5883-4114-A1A3-40EDE66A747B}" name="2. Protoyp fertig" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B2A1622D-5883-4114-A1A3-40EDE66A747B}" name="2. Protoyp fertig" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Outcomes table style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
   <extLst>
@@ -3953,8 +3956,8 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4026,7 +4029,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4060,13 +4063,13 @@
       <c r="F7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="62" t="s">
+      <c r="I7" s="59" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4074,110 +4077,114 @@
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="43" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="56">
         <v>1</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="56">
         <v>9</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="56">
         <v>6</v>
       </c>
-      <c r="G9" s="60">
+      <c r="G9" s="57">
         <v>6</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="58">
         <v>2</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="60">
         <f>SUM(D9:H9)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="59">
+      <c r="D10" s="56">
         <v>1</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="61"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="60">
+        <f>SUM(D10:H10)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="36">
         <v>0.05</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="36">
         <v>0.05</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="36">
         <v>0.05</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="37">
         <v>0.05</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="45">
         <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="50">
+      <c r="D12" s="47">
         <f xml:space="preserve"> D9/2</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="50">
+      <c r="E12" s="47">
         <f xml:space="preserve"> E9/2</f>
         <v>4.5</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="47">
         <f xml:space="preserve"> F9/2</f>
         <v>3</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="48">
         <f xml:space="preserve"> G9/2</f>
         <v>3</v>
       </c>
-      <c r="H12" s="52">
+      <c r="H12" s="49">
         <f xml:space="preserve"> H9/2</f>
         <v>1</v>
       </c>
-      <c r="I12" s="64">
+      <c r="I12" s="61">
         <f>SUM(D12:H12)</f>
         <v>12</v>
       </c>
@@ -4186,110 +4193,114 @@
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="53" t="s">
+      <c r="G13" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="54" t="s">
+      <c r="H13" s="51" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="56">
         <v>1</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="56">
         <v>12</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="56">
         <v>2</v>
       </c>
-      <c r="G14" s="60">
+      <c r="G14" s="57">
         <v>2</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="58">
         <v>3</v>
       </c>
-      <c r="I14" s="63">
+      <c r="I14" s="60">
         <f>SUM(D14:H14)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="59">
+      <c r="D15" s="56">
         <v>1</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="61"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="60">
+        <f>SUM(D15:H15)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="36">
         <v>0.05</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="36">
         <v>0.05</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="36">
         <v>0.05</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="37">
         <v>0.05</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="45">
         <v>0.05</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="47">
         <f xml:space="preserve"> D14/2</f>
         <v>0.5</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="47">
         <f xml:space="preserve"> E14/2</f>
         <v>6</v>
       </c>
-      <c r="F17" s="50">
+      <c r="F17" s="47">
         <f xml:space="preserve"> F14/2</f>
         <v>1</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="48">
         <f xml:space="preserve"> G14/2</f>
         <v>1</v>
       </c>
-      <c r="H17" s="52">
+      <c r="H17" s="49">
         <f xml:space="preserve"> H14/2</f>
         <v>1.5</v>
       </c>
-      <c r="I17" s="64">
+      <c r="I17" s="61">
         <f>SUM(D17:H17)</f>
         <v>10</v>
       </c>
@@ -4298,220 +4309,228 @@
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="46" t="s">
+      <c r="H18" s="43" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="56">
         <v>8</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="56">
         <v>2</v>
       </c>
-      <c r="F19" s="59">
+      <c r="F19" s="56">
         <v>4</v>
       </c>
-      <c r="G19" s="60">
+      <c r="G19" s="57">
         <v>4</v>
       </c>
-      <c r="H19" s="61">
+      <c r="H19" s="58">
         <v>2</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="60">
         <f>SUM(D19:H19)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="56">
         <v>10</v>
       </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="61"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="60">
+        <f>SUM(D20:H20)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="36">
         <v>0.05</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="36">
         <v>0.05</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="36">
         <v>0.05</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="37">
         <v>0.05</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="45">
         <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="47">
         <f xml:space="preserve"> D19/2</f>
         <v>4</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="47">
         <f xml:space="preserve"> E19/2</f>
         <v>1</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="47">
         <f xml:space="preserve"> F19/2</f>
         <v>2</v>
       </c>
-      <c r="G22" s="51">
+      <c r="G22" s="48">
         <f xml:space="preserve"> G19/2</f>
         <v>2</v>
       </c>
-      <c r="H22" s="52">
+      <c r="H22" s="49">
         <f xml:space="preserve"> H19/2</f>
         <v>1</v>
       </c>
-      <c r="I22" s="64">
+      <c r="I22" s="61">
         <f>SUM(D22:H22)</f>
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="57" t="s">
+      <c r="G23" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="55" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="59">
+      <c r="D24" s="56">
         <v>1</v>
       </c>
-      <c r="E24" s="59">
+      <c r="E24" s="56">
         <v>8</v>
       </c>
-      <c r="F24" s="59">
+      <c r="F24" s="56">
         <v>3</v>
       </c>
-      <c r="G24" s="60">
+      <c r="G24" s="57">
         <v>4</v>
       </c>
-      <c r="H24" s="61">
+      <c r="H24" s="58">
         <v>4</v>
       </c>
-      <c r="I24" s="63">
+      <c r="I24" s="60">
         <f>SUM(D24:H24)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="56">
         <v>1</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="61"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="60">
+        <f>SUM(D25:H25)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="36">
         <v>0.05</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="36">
         <v>0.05</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="36">
         <v>0.05</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="37">
         <v>0.05</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="45">
         <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="50">
+      <c r="D27" s="47">
         <f xml:space="preserve"> D24/2</f>
         <v>0.5</v>
       </c>
-      <c r="E27" s="50">
+      <c r="E27" s="47">
         <f xml:space="preserve"> E24/2</f>
         <v>4</v>
       </c>
-      <c r="F27" s="50">
+      <c r="F27" s="47">
         <f xml:space="preserve"> F24/2</f>
         <v>1.5</v>
       </c>
-      <c r="G27" s="51">
+      <c r="G27" s="48">
         <f xml:space="preserve"> G24/2</f>
         <v>2</v>
       </c>
-      <c r="H27" s="52">
+      <c r="H27" s="49">
         <f xml:space="preserve"> H24/2</f>
         <v>2</v>
       </c>
-      <c r="I27" s="64">
+      <c r="I27" s="61">
         <f>SUM(D27:H27)</f>
         <v>10</v>
       </c>
@@ -4586,7 +4605,7 @@
       <c r="G31" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="36" t="s">
+      <c r="H31" s="62" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4609,7 +4628,7 @@
       <c r="G32" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="37"/>
+      <c r="H32" s="63"/>
     </row>
     <row r="33" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="17" t="s">
@@ -4627,7 +4646,7 @@
       <c r="G33" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="37"/>
+      <c r="H33" s="63"/>
     </row>
     <row r="34" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="18" t="s">
@@ -4645,7 +4664,7 @@
       <c r="G34" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="38"/>
+      <c r="H34" s="64"/>
     </row>
     <row r="36" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="23" t="s">

</xml_diff>

<commit_message>
TO DO, ist Zeil einfügen
- Ramon hat das gemacht
</commit_message>
<xml_diff>
--- a/Dokumentation/Terminplan.xlsx
+++ b/Dokumentation/Terminplan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D42D7-1974-4905-A527-CE2BDADDE581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE98781-386E-4DFB-AC52-C9C765A15985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
+    <workbookView xWindow="-98" yWindow="503" windowWidth="20715" windowHeight="13274" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminplan" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -518,13 +516,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="[$-407]d\.\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;Wochen&quot;"/>
-    <numFmt numFmtId="170" formatCode="0\ \ &quot;Stunden&quot;"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="[$-407]d\.\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="0.0\ &quot;Wochen&quot;"/>
+    <numFmt numFmtId="168" formatCode="0\ \ &quot;Stunden&quot;"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1498,10 +1496,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1588,7 +1586,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1629,7 +1627,7 @@
     <xf numFmtId="0" fontId="2" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
@@ -1677,13 +1675,13 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="37" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="37" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="37" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="37" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="37" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1704,22 +1702,22 @@
     <xf numFmtId="0" fontId="2" fillId="34" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="37" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="37" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="37" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1733,53 +1731,53 @@
     </xf>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20 % - Akzent1" xfId="24" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="28" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="32" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="36" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="40" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="44" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="25" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="29" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="33" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="37" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="41" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="45" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="26" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="30" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="34" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="38" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="42" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="46" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="23" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="31" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="35" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="39" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="43" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="15" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="16" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Dezimal [0]" xfId="6" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="14" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="22" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="21" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="11" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="5" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="24" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="28" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="32" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="40" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="44" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="25" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="29" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="33" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="41" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="45" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="26" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="30" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="34" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="38" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="42" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="46" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="23" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="27" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="31" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="39" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="43" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="12" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="5" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="6" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="7" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="8" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="21" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="11" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="4" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="14" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="17" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="13" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="20" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="9" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="12" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Überschrift" xfId="10" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="3" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="4" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="17" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung" xfId="7" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Währung [0]" xfId="8" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="19" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="20" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="9" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="10" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="22" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="19" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -2035,7 +2033,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2136,12 +2134,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21787663-4A21-4442-A1D7-1F1E8A107D74}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{6893A20C-7E17-40DE-84D3-153AD2E13BC3}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2169,12 +2167,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FBF1BAEE-70A3-40A7-8FD5-F944CEE1E780}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{4FB52356-FE67-4B7F-AFBA-FAB09758A452}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2202,12 +2200,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D92D8BA-BA51-41D3-A307-5E6C04F72D3C}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{B9D94F00-244B-48D1-B9F3-46552CC31BB1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2235,12 +2233,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67C62430-54B0-41C1-AB21-F561D122263D}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{56F3B0BD-BB43-4096-8814-1F426E66B749}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2268,12 +2266,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8514844-197C-4B5F-AFA9-C2A738DEB967}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{EC0417BE-8D03-4874-B804-60DC39E9CD99}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2304,9 +2302,9 @@
                     <a:fld id="{EA1BE266-518F-4604-B935-ED891CFF236B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2334,12 +2332,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D46C1F9C-EE3D-462D-850B-C9ED7A618A63}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{5E0D490E-96AB-45FD-A65C-56DF0194B83A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2367,12 +2365,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09B3B258-18AA-4545-A783-28A0D4DFEF62}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{B37BE6D9-C2E8-498F-A9F0-9ED417C7F45A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2409,9 +2407,9 @@
                     <a:fld id="{308EB7F1-46D2-4D1E-958A-AF29BC74DE96}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2438,12 +2436,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C50F171-2994-4F8C-9818-D6E795E1F43F}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{002B80D0-8D81-4FB6-8EC9-7D82130457AB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2480,9 +2478,9 @@
                     <a:fld id="{FFFA1F33-0865-4DEE-B299-9613A07D58E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[ZELLBEREICH]</a:t>
+                      <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-GB"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -3956,23 +3954,23 @@
   </sheetPr>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="46" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.08203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.58203125" customWidth="1"/>
-    <col min="4" max="4" width="64.4140625" customWidth="1"/>
-    <col min="5" max="6" width="40.58203125" customWidth="1"/>
-    <col min="7" max="7" width="43.4140625" customWidth="1"/>
-    <col min="8" max="8" width="29.9140625" customWidth="1"/>
+    <col min="1" max="1" width="3.0625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" customWidth="1"/>
+    <col min="3" max="3" width="40.5625" customWidth="1"/>
+    <col min="4" max="4" width="64.4375" customWidth="1"/>
+    <col min="5" max="6" width="40.5625" customWidth="1"/>
+    <col min="7" max="7" width="43.4375" customWidth="1"/>
+    <col min="8" max="8" width="29.9375" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="55.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="C1" s="6" t="s">
         <v>44</v>
@@ -3983,7 +3981,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="279.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="279.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -3992,7 +3990,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
       <c r="C3" s="35" t="s">
         <v>73</v>
@@ -4005,7 +4003,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -4014,7 +4012,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="85.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
@@ -4029,7 +4027,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4048,7 +4046,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -4073,7 +4071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -4096,7 +4094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
       <c r="C9" s="44" t="s">
         <v>76</v>
@@ -4121,7 +4119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
       <c r="C10" s="44" t="s">
         <v>77</v>
@@ -4129,16 +4127,24 @@
       <c r="D10" s="56">
         <v>1</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="58"/>
+      <c r="E10" s="56">
+        <v>20</v>
+      </c>
+      <c r="F10" s="56">
+        <v>3</v>
+      </c>
+      <c r="G10" s="57">
+        <v>0</v>
+      </c>
+      <c r="H10" s="58">
+        <v>4</v>
+      </c>
       <c r="I10" s="60">
         <f>SUM(D10:H10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="44" t="s">
         <v>78</v>
@@ -4159,7 +4165,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
       <c r="C12" s="46" t="s">
         <v>79</v>
@@ -4189,7 +4195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -4212,7 +4218,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="1"/>
       <c r="C14" s="44" t="s">
         <v>76</v>
@@ -4237,7 +4243,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="1"/>
       <c r="C15" s="44" t="s">
         <v>77</v>
@@ -4254,7 +4260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="44" t="s">
         <v>78</v>
@@ -4275,7 +4281,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="46" t="s">
         <v>79</v>
@@ -4305,7 +4311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="44" t="s">
         <v>76</v>
@@ -4353,7 +4359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="44" t="s">
         <v>77</v>
@@ -4370,7 +4376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="44" t="s">
         <v>78</v>
@@ -4391,7 +4397,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="46" t="s">
         <v>79</v>
@@ -4421,7 +4427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="52" t="s">
         <v>26</v>
@@ -4442,7 +4448,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="44" t="s">
         <v>76</v>
@@ -4467,7 +4473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="44" t="s">
         <v>77</v>
@@ -4484,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="44" t="s">
         <v>78</v>
@@ -4505,7 +4511,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
       <c r="C27" s="46" t="s">
         <v>79</v>
@@ -4535,10 +4541,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
@@ -4562,7 +4568,7 @@
       </c>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
@@ -4586,7 +4592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
@@ -4609,7 +4615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>4</v>
       </c>
@@ -4630,7 +4636,7 @@
       </c>
       <c r="H32" s="63"/>
     </row>
-    <row r="33" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C33" s="17" t="s">
         <v>43</v>
       </c>
@@ -4648,7 +4654,7 @@
       </c>
       <c r="H33" s="63"/>
     </row>
-    <row r="34" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:8" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C34" s="18" t="s">
         <v>26</v>
       </c>
@@ -4666,18 +4672,18 @@
       </c>
       <c r="H34" s="64"/>
     </row>
-    <row r="36" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C36" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C37" s="25" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="24"/>
     </row>
-    <row r="38" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C38" s="26" t="s">
         <v>41</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="39" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C39" s="26" t="s">
         <v>42</v>
       </c>
@@ -4725,7 +4731,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
@@ -4734,14 +4740,14 @@
     <col min="6" max="6" width="21.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:4" ht="34.9" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
@@ -4755,7 +4761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="16">
         <f>DATE(2019,9,26)</f>
         <v>43734</v>
@@ -4770,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="16">
         <v>43746</v>
       </c>
@@ -4784,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="16">
         <f>DATE(2019,10,13)</f>
         <v>43751</v>
@@ -4799,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="16">
         <v>43766</v>
       </c>
@@ -4813,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="16">
         <v>43770</v>
       </c>
@@ -4827,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="16">
         <f>DATE(2019,11,10)</f>
         <v>43779</v>
@@ -4842,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="16">
         <f>DATE(2019,11,14)</f>
         <v>43783</v>
@@ -4857,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="16">
         <f>DATE(2019,11,28)</f>
         <v>43797</v>
@@ -4872,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="16">
         <f>DATE(2019,12,12)</f>
         <v>43811</v>
@@ -4887,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="16">
         <f>DATE(2019,12,19)</f>
         <v>43818</v>
@@ -4902,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="16">
         <f>DATE(2019,12,22)</f>
         <v>43821</v>
@@ -4917,20 +4923,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" s="31"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B18" s="31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zeiten für Michael eingetragen
</commit_message>
<xml_diff>
--- a/Dokumentation/Terminplan.xlsx
+++ b/Dokumentation/Terminplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8231D8F1-F60F-4C24-B5D1-0C34540A76EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04986D81-7029-4434-B2D4-E981EA308E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACC784CE-6BA7-4857-A17F-37B6681AB0C0}"/>
   </bookViews>
@@ -2141,7 +2141,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C2431CB-95C6-4968-9751-78D85CA0C095}" type="CELLRANGE">
+                    <a:fld id="{88C8F550-8331-49A6-A7DA-811F308BE760}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2174,7 +2174,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9479F0FD-E38B-4C94-9682-EFFBA9DBFE20}" type="CELLRANGE">
+                    <a:fld id="{1B824583-8569-444C-B940-66327EA3C88C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2207,7 +2207,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1B39308-2AF4-48A0-9849-F747C05AE9B6}" type="CELLRANGE">
+                    <a:fld id="{45E78D59-92B7-47B7-97CF-3E19A8D41D76}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2240,7 +2240,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A6469FA-9C26-46CD-B253-A6D31AD267A9}" type="CELLRANGE">
+                    <a:fld id="{42B808B1-0C43-4934-9E56-9CB9318FB132}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2273,7 +2273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60432AA8-C27A-443D-A234-E64D5C7437DB}" type="CELLRANGE">
+                    <a:fld id="{12EF7916-8748-4213-9FEE-A1568E3D567F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2339,7 +2339,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76B34BF0-618A-455B-927E-98DE6D2649F7}" type="CELLRANGE">
+                    <a:fld id="{7F1E6CA5-61D2-4D52-A8D4-8229D03C7210}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2372,7 +2372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86298C16-D835-4441-9AC9-3D7C2AA48194}" type="CELLRANGE">
+                    <a:fld id="{8C8C9ECE-8F10-4AF8-9046-E618D1560973}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2443,7 +2443,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DAC759E-42F7-4771-8525-1B3F60551296}" type="CELLRANGE">
+                    <a:fld id="{14908CBB-908A-4852-9E7A-4BBB4BC8039C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -3962,7 +3962,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="46" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4258,13 +4258,21 @@
       <c r="D15" s="56">
         <v>1</v>
       </c>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
+      <c r="E15" s="56">
+        <v>20</v>
+      </c>
+      <c r="F15" s="56">
+        <v>2</v>
+      </c>
+      <c r="G15" s="57">
+        <v>1</v>
+      </c>
+      <c r="H15" s="58">
+        <v>2</v>
+      </c>
       <c r="I15" s="60">
         <f>SUM(D15:H15)</f>
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>